<commit_message>
Resolução dos bugs com as linhas de faturação
</commit_message>
<xml_diff>
--- a/ASSREG-Faturacao/copia.xlsx
+++ b/ASSREG-Faturacao/copia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A9CEAF-915D-437E-8E5F-EAB4CB5E5449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFB2A4C-8742-4790-88EF-61BD027E1062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="804" windowWidth="23556" windowHeight="9948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5352" yWindow="1248" windowWidth="23556" windowHeight="9948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANTAO 1" sheetId="3" r:id="rId1"/>
@@ -284,14 +284,14 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,7 +644,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomLeft" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +654,7 @@
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="34" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="32" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="18" customWidth="1"/>
     <col min="13" max="13" width="46.5546875" customWidth="1"/>
     <col min="14" max="14" width="10.44140625" style="23" bestFit="1" customWidth="1"/>
@@ -665,58 +665,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="31" t="s">
+      <c r="A1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="33" t="s">
         <v>9</v>
       </c>
     </row>
@@ -733,7 +733,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="33"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="17"/>
       <c r="M2" s="3"/>
       <c r="N2" s="22"/>
@@ -743,58 +743,58 @@
       <c r="R2" s="22"/>
     </row>
     <row r="3" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="32" t="s">
+      <c r="A3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
         <v>44888</v>
       </c>
       <c r="R8" s="27">
-        <v>2200</v>
+        <v>22000</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>